<commit_message>
Cell Format and Totals
Updated tracker cell formats and how/where day total is calculated/placed
</commit_message>
<xml_diff>
--- a/HHS Operations/ORIGINALS/Template_MasterRevenueTracker.xlsx
+++ b/HHS Operations/ORIGINALS/Template_MasterRevenueTracker.xlsx
@@ -300,15 +300,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -332,7 +332,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -391,10 +391,10 @@
   <dimension ref="B1:T38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U26" activeCellId="0" sqref="U26"/>
+      <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.81"/>

</xml_diff>